<commit_message>
finished cmc prediction notebook run and new trained model prediction notebook
</commit_message>
<xml_diff>
--- a/v0.2/commercial_models/release_v0.2_20240610/prediction_by_cmcModel_validate.xlsx
+++ b/v0.2/commercial_models/release_v0.2_20240610/prediction_by_cmcModel_validate.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IchorCNA</t>
+          <t>ichorCNA</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -486,7 +486,7 @@
         <v>0.1174242424242424</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9962406015037594</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -557,7 +557,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN</t>
+          <t>ichorCNA,FLEN</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -570,20 +570,20 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IchorCNA,EM</t>
+          <t>ichorCNA,EM</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>0.4090909090909091</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9736842105263158</v>
+        <v>0.9774436090225563</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -596,7 +596,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_FLEN</t>
+          <t>ichorCNA,OT_FLEN</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -609,7 +609,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_NUCLEOSOME</t>
+          <t>ichorCNA,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -622,7 +622,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IchorCNA,NMF_FLEN</t>
+          <t>ichorCNA,NMF_FLEN</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -635,7 +635,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IchorCNA,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -655,7 +655,7 @@
         <v>0.2348484848484849</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8834586466165414</v>
+        <v>0.8872180451127819</v>
       </c>
     </row>
     <row r="18">
@@ -733,7 +733,7 @@
         <v>0.3901515151515151</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7781954887218046</v>
+        <v>0.7819548872180451</v>
       </c>
     </row>
     <row r="24">
@@ -746,7 +746,7 @@
         <v>0.2803030303030303</v>
       </c>
       <c r="C24" t="n">
-        <v>0.6616541353383458</v>
+        <v>0.6654135338345865</v>
       </c>
     </row>
     <row r="25">
@@ -759,7 +759,7 @@
         <v>0.3106060606060606</v>
       </c>
       <c r="C25" t="n">
-        <v>0.6654135338345865</v>
+        <v>0.6691729323308271</v>
       </c>
     </row>
     <row r="26">
@@ -772,7 +772,7 @@
         <v>0.2916666666666667</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9887218045112782</v>
+        <v>0.9924812030075187</v>
       </c>
     </row>
     <row r="27">
@@ -785,7 +785,7 @@
         <v>0.3674242424242424</v>
       </c>
       <c r="C27" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.3609022556390977</v>
       </c>
     </row>
     <row r="28">
@@ -921,20 +921,20 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM</t>
+          <t>ichorCNA,FLEN,EM</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>0.4507575757575757</v>
       </c>
       <c r="C38" t="n">
-        <v>0.8721804511278195</v>
+        <v>0.8759398496240601</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -947,7 +947,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_FLEN</t>
+          <t>ichorCNA,FLEN,OT_FLEN</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -960,7 +960,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -973,7 +973,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,NMF_FLEN</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -986,7 +986,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -999,72 +999,72 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>0.553030303030303</v>
       </c>
       <c r="C44" t="n">
-        <v>0.7706766917293233</v>
+        <v>0.7744360902255639</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_FLEN</t>
+          <t>ichorCNA,EM,OT_FLEN</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>0.4924242424242424</v>
       </c>
       <c r="C45" t="n">
-        <v>0.6541353383458647</v>
+        <v>0.6578947368421053</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_NUCLEOSOME</t>
+          <t>ichorCNA,EM,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>0.5227272727272727</v>
       </c>
       <c r="C46" t="n">
-        <v>0.6654135338345865</v>
+        <v>0.6691729323308271</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NMF_FLEN</t>
+          <t>ichorCNA,EM,NMF_FLEN</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>0.4583333333333333</v>
       </c>
       <c r="C47" t="n">
-        <v>0.9699248120300752</v>
+        <v>0.9736842105263158</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>0.6325757575757576</v>
       </c>
       <c r="C48" t="n">
-        <v>0.3421052631578947</v>
+        <v>0.3458646616541353</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_FLEN</t>
+          <t>ichorCNA,NUCLEOSOME,OT_FLEN</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1077,7 +1077,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1090,7 +1090,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1103,7 +1103,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1116,7 +1116,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_FLEN,OT_NUCLEOSOME</t>
+          <t>ichorCNA,OT_FLEN,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1129,7 +1129,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_FLEN,NMF_FLEN</t>
+          <t>ichorCNA,OT_FLEN,NMF_FLEN</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1142,7 +1142,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,OT_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1155,7 +1155,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1168,7 +1168,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1181,7 +1181,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>IchorCNA,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1201,7 +1201,7 @@
         <v>0.3939393939393939</v>
       </c>
       <c r="C59" t="n">
-        <v>0.7406015037593985</v>
+        <v>0.7443609022556391</v>
       </c>
     </row>
     <row r="60">
@@ -1214,7 +1214,7 @@
         <v>0.2840909090909091</v>
       </c>
       <c r="C60" t="n">
-        <v>0.6578947368421053</v>
+        <v>0.6616541353383458</v>
       </c>
     </row>
     <row r="61">
@@ -1227,7 +1227,7 @@
         <v>0.3143939393939394</v>
       </c>
       <c r="C61" t="n">
-        <v>0.6466165413533834</v>
+        <v>0.6503759398496241</v>
       </c>
     </row>
     <row r="62">
@@ -1240,7 +1240,7 @@
         <v>0.3295454545454545</v>
       </c>
       <c r="C62" t="n">
-        <v>0.8796992481203008</v>
+        <v>0.8834586466165414</v>
       </c>
     </row>
     <row r="63">
@@ -1253,7 +1253,7 @@
         <v>0.4583333333333333</v>
       </c>
       <c r="C63" t="n">
-        <v>0.3421052631578947</v>
+        <v>0.3458646616541353</v>
       </c>
     </row>
     <row r="64">
@@ -1396,7 +1396,7 @@
         <v>0.4090909090909091</v>
       </c>
       <c r="C74" t="n">
-        <v>0.5789473684210527</v>
+        <v>0.5827067669172933</v>
       </c>
     </row>
     <row r="75">
@@ -1409,7 +1409,7 @@
         <v>0.4090909090909091</v>
       </c>
       <c r="C75" t="n">
-        <v>0.6278195488721805</v>
+        <v>0.631578947368421</v>
       </c>
     </row>
     <row r="76">
@@ -1422,7 +1422,7 @@
         <v>0.4431818181818182</v>
       </c>
       <c r="C76" t="n">
-        <v>0.7781954887218046</v>
+        <v>0.7819548872180451</v>
       </c>
     </row>
     <row r="77">
@@ -1435,7 +1435,7 @@
         <v>0.5833333333333334</v>
       </c>
       <c r="C77" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="78">
@@ -1448,7 +1448,7 @@
         <v>0.3446969696969697</v>
       </c>
       <c r="C78" t="n">
-        <v>0.5225563909774437</v>
+        <v>0.5263157894736842</v>
       </c>
     </row>
     <row r="79">
@@ -1461,7 +1461,7 @@
         <v>0.375</v>
       </c>
       <c r="C79" t="n">
-        <v>0.6578947368421053</v>
+        <v>0.6616541353383458</v>
       </c>
     </row>
     <row r="80">
@@ -1474,7 +1474,7 @@
         <v>0.4772727272727273</v>
       </c>
       <c r="C80" t="n">
-        <v>0.3007518796992481</v>
+        <v>0.3045112781954887</v>
       </c>
     </row>
     <row r="81">
@@ -1487,7 +1487,7 @@
         <v>0.4053030303030303</v>
       </c>
       <c r="C81" t="n">
-        <v>0.6616541353383458</v>
+        <v>0.6654135338345865</v>
       </c>
     </row>
     <row r="82">
@@ -1500,7 +1500,7 @@
         <v>0.4924242424242424</v>
       </c>
       <c r="C82" t="n">
-        <v>0.2894736842105263</v>
+        <v>0.2932330827067669</v>
       </c>
     </row>
     <row r="83">
@@ -1513,7 +1513,7 @@
         <v>0.5416666666666666</v>
       </c>
       <c r="C83" t="n">
-        <v>0.3496240601503759</v>
+        <v>0.3533834586466165</v>
       </c>
     </row>
     <row r="84">
@@ -1649,72 +1649,72 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME</t>
         </is>
       </c>
       <c r="B94" t="n">
         <v>0.5568181818181818</v>
       </c>
       <c r="C94" t="n">
-        <v>0.7368421052631579</v>
+        <v>0.7406015037593985</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_FLEN</t>
+          <t>ichorCNA,FLEN,EM,OT_FLEN</t>
         </is>
       </c>
       <c r="B95" t="n">
         <v>0.4924242424242424</v>
       </c>
       <c r="C95" t="n">
-        <v>0.6503759398496241</v>
+        <v>0.6541353383458647</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B96" t="n">
         <v>0.5227272727272727</v>
       </c>
       <c r="C96" t="n">
-        <v>0.6466165413533834</v>
+        <v>0.6503759398496241</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,EM,NMF_FLEN</t>
         </is>
       </c>
       <c r="B97" t="n">
         <v>0.4886363636363636</v>
       </c>
       <c r="C97" t="n">
-        <v>0.868421052631579</v>
+        <v>0.8721804511278195</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B98" t="n">
         <v>0.6477272727272727</v>
       </c>
       <c r="C98" t="n">
-        <v>0.3345864661654135</v>
+        <v>0.3383458646616541</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_FLEN</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_FLEN</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -1727,7 +1727,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -1740,7 +1740,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -1753,7 +1753,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -1766,7 +1766,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_FLEN,OT_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,OT_FLEN,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -1779,7 +1779,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_FLEN,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,OT_FLEN,NMF_FLEN</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -1792,7 +1792,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,OT_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -1805,7 +1805,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -1818,7 +1818,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -1831,7 +1831,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -1844,137 +1844,137 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_FLEN</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_FLEN</t>
         </is>
       </c>
       <c r="B109" t="n">
         <v>0.571969696969697</v>
       </c>
       <c r="C109" t="n">
-        <v>0.575187969924812</v>
+        <v>0.5789473684210527</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B110" t="n">
         <v>0.571969696969697</v>
       </c>
       <c r="C110" t="n">
-        <v>0.6278195488721805</v>
+        <v>0.631578947368421</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,EM,NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B111" t="n">
         <v>0.571969696969697</v>
       </c>
       <c r="C111" t="n">
-        <v>0.7706766917293233</v>
+        <v>0.7744360902255639</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B112" t="n">
         <v>0.7196969696969697</v>
       </c>
       <c r="C112" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_FLEN,OT_NUCLEOSOME</t>
+          <t>ichorCNA,EM,OT_FLEN,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B113" t="n">
         <v>0.5454545454545454</v>
       </c>
       <c r="C113" t="n">
-        <v>0.5225563909774437</v>
+        <v>0.5263157894736842</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_FLEN,NMF_FLEN</t>
+          <t>ichorCNA,EM,OT_FLEN,NMF_FLEN</t>
         </is>
       </c>
       <c r="B114" t="n">
         <v>0.5303030303030303</v>
       </c>
       <c r="C114" t="n">
-        <v>0.6503759398496241</v>
+        <v>0.6541353383458647</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,OT_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B115" t="n">
         <v>0.6628787878787878</v>
       </c>
       <c r="C115" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,EM,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B116" t="n">
         <v>0.5568181818181818</v>
       </c>
       <c r="C116" t="n">
-        <v>0.6616541353383458</v>
+        <v>0.6654135338345865</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B117" t="n">
         <v>0.678030303030303</v>
       </c>
       <c r="C117" t="n">
-        <v>0.2894736842105263</v>
+        <v>0.2932330827067669</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B118" t="n">
         <v>0.6818181818181818</v>
       </c>
       <c r="C118" t="n">
-        <v>0.3383458646616541</v>
+        <v>0.3421052631578947</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -1987,7 +1987,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_FLEN,NMF_FLEN</t>
+          <t>ichorCNA,NUCLEOSOME,OT_FLEN,NMF_FLEN</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -2000,7 +2000,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,OT_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -2013,7 +2013,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -2026,7 +2026,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -2039,7 +2039,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -2052,7 +2052,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -2065,7 +2065,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -2078,7 +2078,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -2091,7 +2091,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -2111,7 +2111,7 @@
         <v>0.4090909090909091</v>
       </c>
       <c r="C129" t="n">
-        <v>0.575187969924812</v>
+        <v>0.5789473684210527</v>
       </c>
     </row>
     <row r="130">
@@ -2124,7 +2124,7 @@
         <v>0.4090909090909091</v>
       </c>
       <c r="C130" t="n">
-        <v>0.6090225563909775</v>
+        <v>0.6127819548872181</v>
       </c>
     </row>
     <row r="131">
@@ -2137,7 +2137,7 @@
         <v>0.446969696969697</v>
       </c>
       <c r="C131" t="n">
-        <v>0.7406015037593985</v>
+        <v>0.7443609022556391</v>
       </c>
     </row>
     <row r="132">
@@ -2150,7 +2150,7 @@
         <v>0.5833333333333334</v>
       </c>
       <c r="C132" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="133">
@@ -2163,7 +2163,7 @@
         <v>0.3446969696969697</v>
       </c>
       <c r="C133" t="n">
-        <v>0.518796992481203</v>
+        <v>0.5225563909774437</v>
       </c>
     </row>
     <row r="134">
@@ -2176,7 +2176,7 @@
         <v>0.375</v>
       </c>
       <c r="C134" t="n">
-        <v>0.6541353383458647</v>
+        <v>0.6578947368421053</v>
       </c>
     </row>
     <row r="135">
@@ -2189,7 +2189,7 @@
         <v>0.4810606060606061</v>
       </c>
       <c r="C135" t="n">
-        <v>0.3007518796992481</v>
+        <v>0.3045112781954887</v>
       </c>
     </row>
     <row r="136">
@@ -2202,7 +2202,7 @@
         <v>0.4053030303030303</v>
       </c>
       <c r="C136" t="n">
-        <v>0.6428571428571429</v>
+        <v>0.6466165413533834</v>
       </c>
     </row>
     <row r="137">
@@ -2215,7 +2215,7 @@
         <v>0.4962121212121212</v>
       </c>
       <c r="C137" t="n">
-        <v>0.2894736842105263</v>
+        <v>0.2932330827067669</v>
       </c>
     </row>
     <row r="138">
@@ -2228,7 +2228,7 @@
         <v>0.553030303030303</v>
       </c>
       <c r="C138" t="n">
-        <v>0.3383458646616541</v>
+        <v>0.3421052631578947</v>
       </c>
     </row>
     <row r="139">
@@ -2371,7 +2371,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="C149" t="n">
-        <v>0.4962406015037594</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="150">
@@ -2384,7 +2384,7 @@
         <v>0.4621212121212121</v>
       </c>
       <c r="C150" t="n">
-        <v>0.5789473684210527</v>
+        <v>0.5827067669172933</v>
       </c>
     </row>
     <row r="151">
@@ -2397,7 +2397,7 @@
         <v>0.5833333333333334</v>
       </c>
       <c r="C151" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="152">
@@ -2410,7 +2410,7 @@
         <v>0.4621212121212121</v>
       </c>
       <c r="C152" t="n">
-        <v>0.6278195488721805</v>
+        <v>0.631578947368421</v>
       </c>
     </row>
     <row r="153">
@@ -2423,7 +2423,7 @@
         <v>0.5833333333333334</v>
       </c>
       <c r="C153" t="n">
-        <v>0.2706766917293233</v>
+        <v>0.2744360902255639</v>
       </c>
     </row>
     <row r="154">
@@ -2436,7 +2436,7 @@
         <v>0.6363636363636364</v>
       </c>
       <c r="C154" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="155">
@@ -2449,7 +2449,7 @@
         <v>0.4318181818181818</v>
       </c>
       <c r="C155" t="n">
-        <v>0.518796992481203</v>
+        <v>0.5225563909774437</v>
       </c>
     </row>
     <row r="156">
@@ -2462,7 +2462,7 @@
         <v>0.5189393939393939</v>
       </c>
       <c r="C156" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="157">
@@ -2475,7 +2475,7 @@
         <v>0.571969696969697</v>
       </c>
       <c r="C157" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="158">
@@ -2488,7 +2488,7 @@
         <v>0.5871212121212122</v>
       </c>
       <c r="C158" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.2894736842105263</v>
       </c>
     </row>
     <row r="159">
@@ -2559,137 +2559,137 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN</t>
         </is>
       </c>
       <c r="B164" t="n">
         <v>0.571969696969697</v>
       </c>
       <c r="C164" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.575187969924812</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B165" t="n">
         <v>0.571969696969697</v>
       </c>
       <c r="C165" t="n">
-        <v>0.6090225563909775</v>
+        <v>0.6127819548872181</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B166" t="n">
         <v>0.5757575757575758</v>
       </c>
       <c r="C166" t="n">
-        <v>0.7368421052631579</v>
+        <v>0.7406015037593985</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B167" t="n">
         <v>0.7196969696969697</v>
       </c>
       <c r="C167" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_FLEN,OT_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,OT_FLEN,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B168" t="n">
         <v>0.5454545454545454</v>
       </c>
       <c r="C168" t="n">
-        <v>0.518796992481203</v>
+        <v>0.5225563909774437</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_FLEN,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,EM,OT_FLEN,NMF_FLEN</t>
         </is>
       </c>
       <c r="B169" t="n">
         <v>0.5303030303030303</v>
       </c>
       <c r="C169" t="n">
-        <v>0.6466165413533834</v>
+        <v>0.6503759398496241</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,OT_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B170" t="n">
         <v>0.6628787878787878</v>
       </c>
       <c r="C170" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,EM,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B171" t="n">
         <v>0.5568181818181818</v>
       </c>
       <c r="C171" t="n">
-        <v>0.6428571428571429</v>
+        <v>0.6466165413533834</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B172" t="n">
         <v>0.678030303030303</v>
       </c>
       <c r="C172" t="n">
-        <v>0.2894736842105263</v>
+        <v>0.2932330827067669</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B173" t="n">
         <v>0.6856060606060606</v>
       </c>
       <c r="C173" t="n">
-        <v>0.3308270676691729</v>
+        <v>0.3345864661654135</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -2702,7 +2702,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_FLEN,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_FLEN,NMF_FLEN</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -2715,7 +2715,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -2728,7 +2728,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -2741,7 +2741,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -2754,7 +2754,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -2767,7 +2767,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -2780,7 +2780,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -2793,7 +2793,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -2806,7 +2806,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -2819,137 +2819,137 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B184" t="n">
         <v>0.5795454545454546</v>
       </c>
       <c r="C184" t="n">
-        <v>0.4962406015037594</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_FLEN,NMF_FLEN</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_FLEN,NMF_FLEN</t>
         </is>
       </c>
       <c r="B185" t="n">
         <v>0.5909090909090909</v>
       </c>
       <c r="C185" t="n">
-        <v>0.575187969924812</v>
+        <v>0.5789473684210527</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B186" t="n">
         <v>0.7196969696969697</v>
       </c>
       <c r="C186" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B187" t="n">
         <v>0.5909090909090909</v>
       </c>
       <c r="C187" t="n">
-        <v>0.6278195488721805</v>
+        <v>0.631578947368421</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B188" t="n">
         <v>0.7196969696969697</v>
       </c>
       <c r="C188" t="n">
-        <v>0.2706766917293233</v>
+        <v>0.2744360902255639</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B189" t="n">
         <v>0.7386363636363636</v>
       </c>
       <c r="C189" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,EM,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B190" t="n">
         <v>0.5795454545454546</v>
       </c>
       <c r="C190" t="n">
-        <v>0.518796992481203</v>
+        <v>0.5225563909774437</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B191" t="n">
         <v>0.6931818181818182</v>
       </c>
       <c r="C191" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B192" t="n">
         <v>0.7007575757575758</v>
       </c>
       <c r="C192" t="n">
-        <v>0.2932330827067669</v>
+        <v>0.2969924812030075</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B193" t="n">
         <v>0.7121212121212122</v>
       </c>
       <c r="C193" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.2894736842105263</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -2962,7 +2962,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -2975,7 +2975,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -2988,7 +2988,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -3001,7 +3001,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>IchorCNA,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -3021,7 +3021,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="C199" t="n">
-        <v>0.4924812030075188</v>
+        <v>0.4962406015037594</v>
       </c>
     </row>
     <row r="200">
@@ -3034,7 +3034,7 @@
         <v>0.4621212121212121</v>
       </c>
       <c r="C200" t="n">
-        <v>0.575187969924812</v>
+        <v>0.5789473684210527</v>
       </c>
     </row>
     <row r="201">
@@ -3047,7 +3047,7 @@
         <v>0.5833333333333334</v>
       </c>
       <c r="C201" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="202">
@@ -3060,7 +3060,7 @@
         <v>0.4621212121212121</v>
       </c>
       <c r="C202" t="n">
-        <v>0.6090225563909775</v>
+        <v>0.6127819548872181</v>
       </c>
     </row>
     <row r="203">
@@ -3073,7 +3073,7 @@
         <v>0.5833333333333334</v>
       </c>
       <c r="C203" t="n">
-        <v>0.2706766917293233</v>
+        <v>0.2744360902255639</v>
       </c>
     </row>
     <row r="204">
@@ -3086,7 +3086,7 @@
         <v>0.6363636363636364</v>
       </c>
       <c r="C204" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="205">
@@ -3099,7 +3099,7 @@
         <v>0.4318181818181818</v>
       </c>
       <c r="C205" t="n">
-        <v>0.5150375939849624</v>
+        <v>0.518796992481203</v>
       </c>
     </row>
     <row r="206">
@@ -3112,7 +3112,7 @@
         <v>0.5189393939393939</v>
       </c>
       <c r="C206" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="207">
@@ -3125,7 +3125,7 @@
         <v>0.571969696969697</v>
       </c>
       <c r="C207" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="208">
@@ -3138,7 +3138,7 @@
         <v>0.5871212121212122</v>
       </c>
       <c r="C208" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.2894736842105263</v>
       </c>
     </row>
     <row r="209">
@@ -3216,7 +3216,7 @@
         <v>0.4696969696969697</v>
       </c>
       <c r="C214" t="n">
-        <v>0.4962406015037594</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="215">
@@ -3229,7 +3229,7 @@
         <v>0.5833333333333334</v>
       </c>
       <c r="C215" t="n">
-        <v>0.2443609022556391</v>
+        <v>0.2481203007518797</v>
       </c>
     </row>
     <row r="216">
@@ -3242,7 +3242,7 @@
         <v>0.6363636363636364</v>
       </c>
       <c r="C216" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="217">
@@ -3255,7 +3255,7 @@
         <v>0.6363636363636364</v>
       </c>
       <c r="C217" t="n">
-        <v>0.2706766917293233</v>
+        <v>0.2744360902255639</v>
       </c>
     </row>
     <row r="218">
@@ -3268,7 +3268,7 @@
         <v>0.6060606060606061</v>
       </c>
       <c r="C218" t="n">
-        <v>0.2593984962406015</v>
+        <v>0.2631578947368421</v>
       </c>
     </row>
     <row r="219">
@@ -3287,137 +3287,137 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B220" t="n">
         <v>0.5795454545454546</v>
       </c>
       <c r="C220" t="n">
-        <v>0.4924812030075188</v>
+        <v>0.4962406015037594</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,NMF_FLEN</t>
         </is>
       </c>
       <c r="B221" t="n">
         <v>0.5909090909090909</v>
       </c>
       <c r="C221" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.575187969924812</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B222" t="n">
         <v>0.7196969696969697</v>
       </c>
       <c r="C222" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B223" t="n">
         <v>0.5909090909090909</v>
       </c>
       <c r="C223" t="n">
-        <v>0.6090225563909775</v>
+        <v>0.6127819548872181</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B224" t="n">
         <v>0.7196969696969697</v>
       </c>
       <c r="C224" t="n">
-        <v>0.2706766917293233</v>
+        <v>0.2744360902255639</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B225" t="n">
         <v>0.7386363636363636</v>
       </c>
       <c r="C225" t="n">
-        <v>0.2969924812030075</v>
+        <v>0.3007518796992481</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,EM,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B226" t="n">
         <v>0.5795454545454546</v>
       </c>
       <c r="C226" t="n">
-        <v>0.5150375939849624</v>
+        <v>0.518796992481203</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B227" t="n">
         <v>0.6931818181818182</v>
       </c>
       <c r="C227" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B228" t="n">
         <v>0.7007575757575758</v>
       </c>
       <c r="C228" t="n">
-        <v>0.2932330827067669</v>
+        <v>0.2969924812030075</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B229" t="n">
         <v>0.7121212121212122</v>
       </c>
       <c r="C229" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.2894736842105263</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B230" t="n">
@@ -3430,7 +3430,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B231" t="n">
@@ -3443,7 +3443,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -3456,7 +3456,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B233" t="n">
@@ -3469,7 +3469,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -3482,72 +3482,72 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B235" t="n">
         <v>0.5984848484848485</v>
       </c>
       <c r="C235" t="n">
-        <v>0.4962406015037594</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B236" t="n">
         <v>0.7196969696969697</v>
       </c>
       <c r="C236" t="n">
-        <v>0.2443609022556391</v>
+        <v>0.2481203007518797</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B237" t="n">
         <v>0.7386363636363636</v>
       </c>
       <c r="C237" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B238" t="n">
         <v>0.7386363636363636</v>
       </c>
       <c r="C238" t="n">
-        <v>0.2706766917293233</v>
+        <v>0.2744360902255639</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B239" t="n">
         <v>0.7272727272727273</v>
       </c>
       <c r="C239" t="n">
-        <v>0.2593984962406015</v>
+        <v>0.2631578947368421</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>IchorCNA,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B240" t="n">
@@ -3567,7 +3567,7 @@
         <v>0.4696969696969697</v>
       </c>
       <c r="C241" t="n">
-        <v>0.4924812030075188</v>
+        <v>0.4962406015037594</v>
       </c>
     </row>
     <row r="242">
@@ -3580,7 +3580,7 @@
         <v>0.5833333333333334</v>
       </c>
       <c r="C242" t="n">
-        <v>0.2443609022556391</v>
+        <v>0.2481203007518797</v>
       </c>
     </row>
     <row r="243">
@@ -3593,7 +3593,7 @@
         <v>0.6363636363636364</v>
       </c>
       <c r="C243" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="244">
@@ -3606,7 +3606,7 @@
         <v>0.6363636363636364</v>
       </c>
       <c r="C244" t="n">
-        <v>0.2706766917293233</v>
+        <v>0.2744360902255639</v>
       </c>
     </row>
     <row r="245">
@@ -3619,7 +3619,7 @@
         <v>0.6060606060606061</v>
       </c>
       <c r="C245" t="n">
-        <v>0.2593984962406015</v>
+        <v>0.2631578947368421</v>
       </c>
     </row>
     <row r="246">
@@ -3645,78 +3645,78 @@
         <v>0.6363636363636364</v>
       </c>
       <c r="C247" t="n">
-        <v>0.2443609022556391</v>
+        <v>0.2481203007518797</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN</t>
         </is>
       </c>
       <c r="B248" t="n">
         <v>0.5984848484848485</v>
       </c>
       <c r="C248" t="n">
-        <v>0.4924812030075188</v>
+        <v>0.4962406015037594</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B249" t="n">
         <v>0.7196969696969697</v>
       </c>
       <c r="C249" t="n">
-        <v>0.2443609022556391</v>
+        <v>0.2481203007518797</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B250" t="n">
         <v>0.7386363636363636</v>
       </c>
       <c r="C250" t="n">
-        <v>0.2631578947368421</v>
+        <v>0.2669172932330827</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B251" t="n">
         <v>0.7386363636363636</v>
       </c>
       <c r="C251" t="n">
-        <v>0.2706766917293233</v>
+        <v>0.2744360902255639</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B252" t="n">
         <v>0.7272727272727273</v>
       </c>
       <c r="C252" t="n">
-        <v>0.2593984962406015</v>
+        <v>0.2631578947368421</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B253" t="n">
@@ -3729,14 +3729,14 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>IchorCNA,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B254" t="n">
         <v>0.7386363636363636</v>
       </c>
       <c r="C254" t="n">
-        <v>0.2443609022556391</v>
+        <v>0.2481203007518797</v>
       </c>
     </row>
     <row r="255">
@@ -3749,20 +3749,20 @@
         <v>0.6363636363636364</v>
       </c>
       <c r="C255" t="n">
-        <v>0.2443609022556391</v>
+        <v>0.2481203007518797</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>IchorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
+          <t>ichorCNA,FLEN,EM,NUCLEOSOME,OT_FLEN,OT_NUCLEOSOME,NMF_FLEN,NMF_NUCLEOSOME</t>
         </is>
       </c>
       <c r="B256" t="n">
         <v>0.7386363636363636</v>
       </c>
       <c r="C256" t="n">
-        <v>0.2443609022556391</v>
+        <v>0.2481203007518797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>